<commit_message>
30.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/May/All Details/23.05.2020/MC Balance Transfer May 2020.xlsx
+++ b/2020/May/All Details/23.05.2020/MC Balance Transfer May 2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -325,6 +325,21 @@
   </si>
   <si>
     <t>Salary May'2020 Murad</t>
+  </si>
+  <si>
+    <t>30.05.2020</t>
+  </si>
+  <si>
+    <t>Bhuiyan</t>
+  </si>
+  <si>
+    <t>Shohel</t>
+  </si>
+  <si>
+    <t>Satata B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apurbo </t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1159,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1156,7 +1171,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1179,14 +1194,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1494,9 +1509,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3143,13 +3158,15 @@
       <c r="B23" s="2">
         <v>173275</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>213545</v>
+      </c>
       <c r="D23" s="2">
         <v>2360</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="0"/>
-        <v>2360</v>
+        <v>215905</v>
       </c>
       <c r="F23" s="96"/>
       <c r="G23" s="80"/>
@@ -3211,13 +3228,21 @@
       <c r="BI23" s="7"/>
     </row>
     <row r="24" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A24" s="14"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1398430</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1252885</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1990</v>
+      </c>
       <c r="E24" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1254875</v>
       </c>
       <c r="F24" s="96"/>
       <c r="G24" s="80"/>
@@ -3826,23 +3851,23 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>10606290</v>
+        <v>12004720</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>10336374</v>
+        <v>11802804</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>100310</v>
+        <v>102300</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>10436684</v>
+        <v>11905104</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>
-        <v>169606</v>
+        <v>99616</v>
       </c>
       <c r="G33" s="82"/>
       <c r="H33" s="87"/>
@@ -4043,11 +4068,11 @@
       </c>
       <c r="E36" s="115">
         <f>F33-C98+K121</f>
-        <v>213545</v>
+        <v>0</v>
       </c>
       <c r="F36" s="63">
         <f>F33-C98-I43-I42+K121-C103</f>
-        <v>213545</v>
+        <v>0</v>
       </c>
       <c r="G36" s="82"/>
       <c r="H36" s="87"/>
@@ -4991,10 +5016,10 @@
       </c>
       <c r="B50" s="30"/>
       <c r="C50" s="71">
-        <v>100000</v>
+        <v>99000</v>
       </c>
       <c r="D50" s="130" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="110"/>
@@ -5128,10 +5153,10 @@
       </c>
       <c r="B52" s="30"/>
       <c r="C52" s="71">
-        <v>194630</v>
+        <v>194520</v>
       </c>
       <c r="D52" s="130" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="110"/>
@@ -5197,10 +5222,10 @@
       </c>
       <c r="B53" s="70"/>
       <c r="C53" s="75">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D53" s="72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="49"/>
@@ -6498,10 +6523,16 @@
       <c r="BI70" s="7"/>
     </row>
     <row r="71" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A71" s="74"/>
+      <c r="A71" s="74" t="s">
+        <v>102</v>
+      </c>
       <c r="B71" s="30"/>
-      <c r="C71" s="71"/>
-      <c r="D71" s="76"/>
+      <c r="C71" s="71">
+        <v>114460</v>
+      </c>
+      <c r="D71" s="76" t="s">
+        <v>101</v>
+      </c>
       <c r="E71" s="6"/>
       <c r="F71" s="111"/>
       <c r="G71" s="13"/>
@@ -6566,10 +6597,16 @@
       <c r="BI71" s="7"/>
     </row>
     <row r="72" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A72" s="73"/>
+      <c r="A72" s="73" t="s">
+        <v>103</v>
+      </c>
       <c r="B72" s="30"/>
-      <c r="C72" s="71"/>
-      <c r="D72" s="76"/>
+      <c r="C72" s="71">
+        <v>28000</v>
+      </c>
+      <c r="D72" s="76" t="s">
+        <v>101</v>
+      </c>
       <c r="E72" s="6"/>
       <c r="F72" s="111"/>
       <c r="G72" s="24" t="s">
@@ -6640,10 +6677,16 @@
       <c r="BI72" s="7"/>
     </row>
     <row r="73" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A73" s="73"/>
+      <c r="A73" s="73" t="s">
+        <v>104</v>
+      </c>
       <c r="B73" s="30"/>
-      <c r="C73" s="71"/>
-      <c r="D73" s="76"/>
+      <c r="C73" s="71">
+        <v>1525</v>
+      </c>
+      <c r="D73" s="76" t="s">
+        <v>101</v>
+      </c>
       <c r="E73" s="6"/>
       <c r="F73" s="111"/>
       <c r="G73" s="13"/>
@@ -6706,10 +6749,16 @@
       <c r="BI73" s="7"/>
     </row>
     <row r="74" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A74" s="73"/>
+      <c r="A74" s="73" t="s">
+        <v>105</v>
+      </c>
       <c r="B74" s="30"/>
-      <c r="C74" s="71"/>
-      <c r="D74" s="70"/>
+      <c r="C74" s="71">
+        <v>10680</v>
+      </c>
+      <c r="D74" s="70" t="s">
+        <v>101</v>
+      </c>
       <c r="E74" s="6"/>
       <c r="F74" s="111"/>
       <c r="G74" s="13" t="s">
@@ -8482,7 +8531,7 @@
       <c r="B98" s="145"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>1582095</v>
+        <v>1725650</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="111"/>
@@ -8617,7 +8666,7 @@
       <c r="B100" s="143"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>1582095</v>
+        <v>1725650</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>